<commit_message>
Updated GUI with Embedded Graphs
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanniebarskhian/Documents/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DFD9F4-6AD2-9D47-826B-BC4280A45248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFDD562-CFF3-0C4E-8DBA-04A63F800A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49180" yWindow="-9560" windowWidth="28320" windowHeight="20680" activeTab="1" xr2:uid="{0F513EA4-1090-9046-8165-4B6792FD4218}"/>
+    <workbookView xWindow="-35780" yWindow="-3140" windowWidth="28320" windowHeight="20680" firstSheet="5" activeTab="19" xr2:uid="{0F513EA4-1090-9046-8165-4B6792FD4218}"/>
   </bookViews>
   <sheets>
     <sheet name="AAPL21" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{7F9BC3CD-3B4F-7944-9C8E-D18398309E36}" name="gldstock" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/fanniebarskhian/Documents/Python/gldstock.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/fanniebarskhian/Documents/Python/gldstock.csv" tab="0" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -12260,7 +12260,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12798,6 +12798,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
       <c r="B24" s="2">
         <v>52.409999847412102</v>
       </c>
@@ -13477,8 +13480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BFDDBC-22DF-B44D-841E-5F5E0447E555}">
   <dimension ref="A1:G254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19340,8 +19343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB52891-FC22-2548-A0B5-BC81212D4BB6}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19819,7 +19822,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20294,7 +20297,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20815,636 +20818,566 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD5C190-41A7-0D48-8957-98929FB36EC9}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>31</v>
       </c>
-      <c r="B2" s="3">
-        <v>44286.270833333336</v>
+      <c r="B2" s="2">
+        <v>121.650001525878</v>
       </c>
       <c r="C2" s="2">
-        <v>121.650001525878</v>
+        <v>123.51999664306599</v>
       </c>
       <c r="D2" s="2">
-        <v>123.51999664306599</v>
+        <v>121.150001525878</v>
       </c>
       <c r="E2" s="2">
-        <v>121.150001525878</v>
+        <v>122.150001525878</v>
       </c>
       <c r="F2" s="2">
-        <v>122.150001525878</v>
+        <v>118323800</v>
       </c>
       <c r="G2" s="2">
-        <v>118323800</v>
-      </c>
-      <c r="H2" s="2">
         <v>121.94287109375</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>30</v>
       </c>
-      <c r="B3" s="3">
-        <v>44285.270833333336</v>
+      <c r="B3" s="2">
+        <v>120.11000061035099</v>
       </c>
       <c r="C3" s="2">
-        <v>120.11000061035099</v>
+        <v>120.400001525878</v>
       </c>
       <c r="D3" s="2">
-        <v>120.400001525878</v>
+        <v>118.86000061035099</v>
       </c>
       <c r="E3" s="2">
-        <v>118.86000061035099</v>
+        <v>119.900001525878</v>
       </c>
       <c r="F3" s="2">
-        <v>119.900001525878</v>
+        <v>85671900</v>
       </c>
       <c r="G3" s="2">
-        <v>85671900</v>
-      </c>
-      <c r="H3" s="2">
         <v>119.696685791015</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>29</v>
       </c>
-      <c r="B4" s="3">
-        <v>44284.270833333336</v>
+      <c r="B4" s="2">
+        <v>121.650001525878</v>
       </c>
       <c r="C4" s="2">
-        <v>121.650001525878</v>
+        <v>122.58000183105401</v>
       </c>
       <c r="D4" s="2">
-        <v>122.58000183105401</v>
+        <v>120.730003356933</v>
       </c>
       <c r="E4" s="2">
-        <v>120.730003356933</v>
+        <v>121.389999389648</v>
       </c>
       <c r="F4" s="2">
-        <v>121.389999389648</v>
+        <v>80819200</v>
       </c>
       <c r="G4" s="2">
-        <v>80819200</v>
-      </c>
-      <c r="H4" s="2">
         <v>121.184158325195</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>26</v>
       </c>
-      <c r="B5" s="3">
-        <v>44281.270833333336</v>
+      <c r="B5" s="2">
+        <v>120.34999847412099</v>
       </c>
       <c r="C5" s="2">
-        <v>120.34999847412099</v>
+        <v>121.480003356933</v>
       </c>
       <c r="D5" s="2">
-        <v>121.480003356933</v>
+        <v>118.919998168945</v>
       </c>
       <c r="E5" s="2">
-        <v>118.919998168945</v>
+        <v>121.209999084472</v>
       </c>
       <c r="F5" s="2">
-        <v>121.209999084472</v>
+        <v>94071200</v>
       </c>
       <c r="G5" s="2">
-        <v>94071200</v>
-      </c>
-      <c r="H5" s="2">
         <v>121.0044631958</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>25</v>
       </c>
-      <c r="B6" s="3">
-        <v>44280.270833333336</v>
+      <c r="B6" s="2">
+        <v>119.540000915527</v>
       </c>
       <c r="C6" s="2">
-        <v>119.540000915527</v>
+        <v>121.66000366210901</v>
       </c>
       <c r="D6" s="2">
-        <v>121.66000366210901</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2">
-        <v>119</v>
+        <v>120.58999633789</v>
       </c>
       <c r="F6" s="2">
-        <v>120.58999633789</v>
+        <v>98844700</v>
       </c>
       <c r="G6" s="2">
-        <v>98844700</v>
-      </c>
-      <c r="H6" s="2">
         <v>120.38551330566401</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
-      <c r="B7" s="3">
-        <v>44279.270833333336</v>
+      <c r="B7" s="2">
+        <v>122.81999969482401</v>
       </c>
       <c r="C7" s="2">
-        <v>122.81999969482401</v>
+        <v>122.900001525878</v>
       </c>
       <c r="D7" s="2">
-        <v>122.900001525878</v>
+        <v>120.06999969482401</v>
       </c>
       <c r="E7" s="2">
-        <v>120.06999969482401</v>
+        <v>120.08999633789</v>
       </c>
       <c r="F7" s="2">
-        <v>120.08999633789</v>
+        <v>88530500</v>
       </c>
       <c r="G7" s="2">
-        <v>88530500</v>
-      </c>
-      <c r="H7" s="2">
         <v>119.886360168457</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>23</v>
       </c>
-      <c r="B8" s="3">
-        <v>44278.270833333336</v>
+      <c r="B8" s="2">
+        <v>123.33000183105401</v>
       </c>
       <c r="C8" s="2">
-        <v>123.33000183105401</v>
+        <v>124.23999786376901</v>
       </c>
       <c r="D8" s="2">
-        <v>124.23999786376901</v>
+        <v>122.139999389648</v>
       </c>
       <c r="E8" s="2">
-        <v>122.139999389648</v>
+        <v>122.540000915527</v>
       </c>
       <c r="F8" s="2">
-        <v>122.540000915527</v>
+        <v>95467100</v>
       </c>
       <c r="G8" s="2">
-        <v>95467100</v>
-      </c>
-      <c r="H8" s="2">
         <v>122.332214355468</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>22</v>
       </c>
-      <c r="B9" s="3">
-        <v>44277.270833333336</v>
+      <c r="B9" s="2">
+        <v>120.33000183105401</v>
       </c>
       <c r="C9" s="2">
-        <v>120.33000183105401</v>
+        <v>123.870002746582</v>
       </c>
       <c r="D9" s="2">
-        <v>123.870002746582</v>
+        <v>120.26000213623</v>
       </c>
       <c r="E9" s="2">
-        <v>120.26000213623</v>
+        <v>123.389999389648</v>
       </c>
       <c r="F9" s="2">
-        <v>123.389999389648</v>
+        <v>111912300</v>
       </c>
       <c r="G9" s="2">
-        <v>111912300</v>
-      </c>
-      <c r="H9" s="2">
         <v>123.180770874023</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
-        <v>44274.270833333336</v>
+      <c r="B10" s="2">
+        <v>119.900001525878</v>
       </c>
       <c r="C10" s="2">
-        <v>119.900001525878</v>
+        <v>121.430000305175</v>
       </c>
       <c r="D10" s="2">
-        <v>121.430000305175</v>
+        <v>119.680000305175</v>
       </c>
       <c r="E10" s="2">
-        <v>119.680000305175</v>
+        <v>119.98999786376901</v>
       </c>
       <c r="F10" s="2">
-        <v>119.98999786376901</v>
+        <v>185549500</v>
       </c>
       <c r="G10" s="2">
-        <v>185549500</v>
-      </c>
-      <c r="H10" s="2">
         <v>119.786529541015</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
-      <c r="B11" s="3">
-        <v>44273.270833333336</v>
+      <c r="B11" s="2">
+        <v>122.879997253417</v>
       </c>
       <c r="C11" s="2">
-        <v>122.879997253417</v>
+        <v>123.180000305175</v>
       </c>
       <c r="D11" s="2">
-        <v>123.180000305175</v>
+        <v>120.31999969482401</v>
       </c>
       <c r="E11" s="2">
-        <v>120.31999969482401</v>
+        <v>120.52999877929599</v>
       </c>
       <c r="F11" s="2">
-        <v>120.52999877929599</v>
+        <v>121229700</v>
       </c>
       <c r="G11" s="2">
-        <v>121229700</v>
-      </c>
-      <c r="H11" s="2">
         <v>120.32561492919901</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>17</v>
       </c>
-      <c r="B12" s="3">
-        <v>44272.270833333336</v>
+      <c r="B12" s="2">
+        <v>124.050003051757</v>
       </c>
       <c r="C12" s="2">
-        <v>124.050003051757</v>
+        <v>125.86000061035099</v>
       </c>
       <c r="D12" s="2">
-        <v>125.86000061035099</v>
+        <v>122.33999633789</v>
       </c>
       <c r="E12" s="2">
-        <v>122.33999633789</v>
+        <v>124.76000213623</v>
       </c>
       <c r="F12" s="2">
-        <v>124.76000213623</v>
+        <v>111932600</v>
       </c>
       <c r="G12" s="2">
-        <v>111932600</v>
-      </c>
-      <c r="H12" s="2">
         <v>124.548446655273</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
-        <v>44271.270833333336</v>
+      <c r="B13" s="2">
+        <v>125.699996948242</v>
       </c>
       <c r="C13" s="2">
-        <v>125.699996948242</v>
+        <v>127.220001220703</v>
       </c>
       <c r="D13" s="2">
-        <v>127.220001220703</v>
+        <v>124.720001220703</v>
       </c>
       <c r="E13" s="2">
-        <v>124.720001220703</v>
+        <v>125.56999969482401</v>
       </c>
       <c r="F13" s="2">
-        <v>125.56999969482401</v>
+        <v>115227900</v>
       </c>
       <c r="G13" s="2">
-        <v>115227900</v>
-      </c>
-      <c r="H13" s="2">
         <v>125.35707092285099</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>15</v>
       </c>
-      <c r="B14" s="3">
-        <v>44270.270833333336</v>
+      <c r="B14" s="2">
+        <v>121.41000366210901</v>
       </c>
       <c r="C14" s="2">
-        <v>121.41000366210901</v>
+        <v>124</v>
       </c>
       <c r="D14" s="2">
-        <v>124</v>
+        <v>120.419998168945</v>
       </c>
       <c r="E14" s="2">
-        <v>120.419998168945</v>
+        <v>123.98999786376901</v>
       </c>
       <c r="F14" s="2">
-        <v>123.98999786376901</v>
+        <v>92403800</v>
       </c>
       <c r="G14" s="2">
-        <v>92403800</v>
-      </c>
-      <c r="H14" s="2">
         <v>123.779747009277</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="3">
-        <v>44267.270833333336</v>
+      <c r="B15" s="2">
+        <v>120.400001525878</v>
       </c>
       <c r="C15" s="2">
-        <v>120.400001525878</v>
+        <v>121.169998168945</v>
       </c>
       <c r="D15" s="2">
-        <v>121.169998168945</v>
+        <v>119.16000366210901</v>
       </c>
       <c r="E15" s="2">
-        <v>119.16000366210901</v>
+        <v>121.02999877929599</v>
       </c>
       <c r="F15" s="2">
-        <v>121.02999877929599</v>
+        <v>88105100</v>
       </c>
       <c r="G15" s="2">
-        <v>88105100</v>
-      </c>
-      <c r="H15" s="2">
         <v>120.82476806640599</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>11</v>
       </c>
-      <c r="B16" s="3">
-        <v>44266.270833333336</v>
+      <c r="B16" s="2">
+        <v>122.540000915527</v>
       </c>
       <c r="C16" s="2">
-        <v>122.540000915527</v>
+        <v>123.209999084472</v>
       </c>
       <c r="D16" s="2">
-        <v>123.209999084472</v>
+        <v>121.26000213623</v>
       </c>
       <c r="E16" s="2">
-        <v>121.26000213623</v>
+        <v>121.959999084472</v>
       </c>
       <c r="F16" s="2">
-        <v>121.959999084472</v>
+        <v>103026500</v>
       </c>
       <c r="G16" s="2">
-        <v>103026500</v>
-      </c>
-      <c r="H16" s="2">
         <v>121.75318908691401</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="B17" s="3">
-        <v>44265.270833333336</v>
+      <c r="B17" s="2">
+        <v>121.69000244140599</v>
       </c>
       <c r="C17" s="2">
-        <v>121.69000244140599</v>
+        <v>122.169998168945</v>
       </c>
       <c r="D17" s="2">
-        <v>122.169998168945</v>
+        <v>119.449996948242</v>
       </c>
       <c r="E17" s="2">
-        <v>119.449996948242</v>
+        <v>119.980003356933</v>
       </c>
       <c r="F17" s="2">
-        <v>119.980003356933</v>
+        <v>111943300</v>
       </c>
       <c r="G17" s="2">
-        <v>111943300</v>
-      </c>
-      <c r="H17" s="2">
         <v>119.776557922363</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
-      <c r="B18" s="3">
-        <v>44264.270833333336</v>
+      <c r="B18" s="2">
+        <v>119.02999877929599</v>
       </c>
       <c r="C18" s="2">
-        <v>119.02999877929599</v>
+        <v>122.059997558593</v>
       </c>
       <c r="D18" s="2">
-        <v>122.059997558593</v>
+        <v>118.790000915527</v>
       </c>
       <c r="E18" s="2">
-        <v>118.790000915527</v>
+        <v>121.08999633789</v>
       </c>
       <c r="F18" s="2">
-        <v>121.08999633789</v>
+        <v>129525800</v>
       </c>
       <c r="G18" s="2">
-        <v>129525800</v>
-      </c>
-      <c r="H18" s="2">
         <v>120.88466644287099</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
-      <c r="B19" s="3">
-        <v>44263.270833333336</v>
+      <c r="B19" s="2">
+        <v>120.930000305175</v>
       </c>
       <c r="C19" s="2">
-        <v>120.930000305175</v>
+        <v>121</v>
       </c>
       <c r="D19" s="2">
-        <v>121</v>
+        <v>116.209999084472</v>
       </c>
       <c r="E19" s="2">
-        <v>116.209999084472</v>
+        <v>116.36000061035099</v>
       </c>
       <c r="F19" s="2">
-        <v>116.36000061035099</v>
+        <v>154376600</v>
       </c>
       <c r="G19" s="2">
-        <v>154376600</v>
-      </c>
-      <c r="H19" s="2">
         <v>116.16268920898401</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
-      <c r="B20" s="3">
-        <v>44260.270833333336</v>
+      <c r="B20" s="2">
+        <v>120.980003356933</v>
       </c>
       <c r="C20" s="2">
-        <v>120.980003356933</v>
+        <v>121.94000244140599</v>
       </c>
       <c r="D20" s="2">
-        <v>121.94000244140599</v>
+        <v>117.56999969482401</v>
       </c>
       <c r="E20" s="2">
-        <v>117.56999969482401</v>
+        <v>121.419998168945</v>
       </c>
       <c r="F20" s="2">
-        <v>121.419998168945</v>
+        <v>153766600</v>
       </c>
       <c r="G20" s="2">
-        <v>153766600</v>
-      </c>
-      <c r="H20" s="2">
         <v>121.21410369873</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
-      <c r="B21" s="3">
-        <v>44259.270833333336</v>
+      <c r="B21" s="2">
+        <v>121.75</v>
       </c>
       <c r="C21" s="2">
-        <v>121.75</v>
+        <v>123.59999847412099</v>
       </c>
       <c r="D21" s="2">
-        <v>123.59999847412099</v>
+        <v>118.620002746582</v>
       </c>
       <c r="E21" s="2">
-        <v>118.620002746582</v>
+        <v>120.129997253417</v>
       </c>
       <c r="F21" s="2">
-        <v>120.129997253417</v>
+        <v>178155000</v>
       </c>
       <c r="G21" s="2">
-        <v>178155000</v>
-      </c>
-      <c r="H21" s="2">
         <v>119.926292419433</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
-      <c r="B22" s="3">
-        <v>44258.270833333336</v>
+      <c r="B22" s="2">
+        <v>124.809997558593</v>
       </c>
       <c r="C22" s="2">
-        <v>124.809997558593</v>
+        <v>125.709999084472</v>
       </c>
       <c r="D22" s="2">
-        <v>125.709999084472</v>
+        <v>121.83999633789</v>
       </c>
       <c r="E22" s="2">
-        <v>121.83999633789</v>
+        <v>122.059997558593</v>
       </c>
       <c r="F22" s="2">
-        <v>122.059997558593</v>
+        <v>112966300</v>
       </c>
       <c r="G22" s="2">
-        <v>112966300</v>
-      </c>
-      <c r="H22" s="2">
         <v>121.853019714355</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23" s="3">
-        <v>44257.270833333336</v>
+      <c r="B23" s="2">
+        <v>128.41000366210901</v>
       </c>
       <c r="C23" s="2">
-        <v>128.41000366210901</v>
+        <v>128.72000122070301</v>
       </c>
       <c r="D23" s="2">
-        <v>128.72000122070301</v>
+        <v>125.01000213623</v>
       </c>
       <c r="E23" s="2">
-        <v>125.01000213623</v>
+        <v>125.120002746582</v>
       </c>
       <c r="F23" s="2">
-        <v>125.120002746582</v>
+        <v>102260900</v>
       </c>
       <c r="G23" s="2">
-        <v>102260900</v>
-      </c>
-      <c r="H23" s="2">
         <v>124.907836914062</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="3">
-        <v>44256.270833333336</v>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2">
+        <v>123.75</v>
       </c>
       <c r="C24" s="2">
-        <v>123.75</v>
+        <v>127.930000305175</v>
       </c>
       <c r="D24" s="2">
-        <v>127.930000305175</v>
+        <v>122.790000915527</v>
       </c>
       <c r="E24" s="2">
-        <v>122.790000915527</v>
+        <v>127.790000915527</v>
       </c>
       <c r="F24" s="2">
-        <v>127.790000915527</v>
+        <v>116307900</v>
       </c>
       <c r="G24" s="2">
-        <v>116307900</v>
-      </c>
-      <c r="H24" s="2">
         <v>127.57331085205</v>
       </c>
     </row>
@@ -21458,7 +21391,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21934,535 +21867,474 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C107283-B31C-8949-8AD6-9080257361AC}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>29</v>
       </c>
-      <c r="B2" s="3">
-        <v>44225.270833333336</v>
+      <c r="B2" s="2">
+        <v>135.83000183105401</v>
       </c>
       <c r="C2" s="2">
-        <v>135.83000183105401</v>
+        <v>136.74000549316401</v>
       </c>
       <c r="D2" s="2">
-        <v>136.74000549316401</v>
+        <v>130.21000671386699</v>
       </c>
       <c r="E2" s="2">
-        <v>130.21000671386699</v>
+        <v>131.96000671386699</v>
       </c>
       <c r="F2" s="2">
-        <v>131.96000671386699</v>
+        <v>177523800</v>
       </c>
       <c r="G2" s="2">
-        <v>177523800</v>
-      </c>
-      <c r="H2" s="2">
         <v>131.53967285156199</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>28</v>
       </c>
-      <c r="B3" s="3">
-        <v>44224.270833333336</v>
+      <c r="B3" s="2">
+        <v>139.52000427246</v>
       </c>
       <c r="C3" s="2">
-        <v>139.52000427246</v>
+        <v>141.99000549316401</v>
       </c>
       <c r="D3" s="2">
-        <v>141.99000549316401</v>
+        <v>136.69999694824199</v>
       </c>
       <c r="E3" s="2">
-        <v>136.69999694824199</v>
+        <v>137.08999633789</v>
       </c>
       <c r="F3" s="2">
-        <v>137.08999633789</v>
+        <v>142621100</v>
       </c>
       <c r="G3" s="2">
-        <v>142621100</v>
-      </c>
-      <c r="H3" s="2">
         <v>136.65333557128901</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>27</v>
       </c>
-      <c r="B4" s="3">
-        <v>44223.270833333336</v>
+      <c r="B4" s="2">
+        <v>143.42999267578099</v>
       </c>
       <c r="C4" s="2">
-        <v>143.42999267578099</v>
+        <v>144.30000305175699</v>
       </c>
       <c r="D4" s="2">
-        <v>144.30000305175699</v>
+        <v>140.41000366210901</v>
       </c>
       <c r="E4" s="2">
-        <v>140.41000366210901</v>
+        <v>142.05999755859301</v>
       </c>
       <c r="F4" s="2">
-        <v>142.05999755859301</v>
+        <v>140843800</v>
       </c>
       <c r="G4" s="2">
-        <v>140843800</v>
-      </c>
-      <c r="H4" s="2">
         <v>141.60751342773401</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>26</v>
       </c>
-      <c r="B5" s="3">
-        <v>44222.270833333336</v>
+      <c r="B5" s="2">
+        <v>143.600006103515</v>
       </c>
       <c r="C5" s="2">
-        <v>143.600006103515</v>
+        <v>144.30000305175699</v>
       </c>
       <c r="D5" s="2">
-        <v>144.30000305175699</v>
+        <v>141.36999511718699</v>
       </c>
       <c r="E5" s="2">
-        <v>141.36999511718699</v>
+        <v>143.16000366210901</v>
       </c>
       <c r="F5" s="2">
-        <v>143.16000366210901</v>
+        <v>98390600</v>
       </c>
       <c r="G5" s="2">
-        <v>98390600</v>
-      </c>
-      <c r="H5" s="2">
         <v>142.704010009765</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>25</v>
       </c>
-      <c r="B6" s="3">
-        <v>44221.270833333336</v>
+      <c r="B6" s="2">
+        <v>143.07000732421801</v>
       </c>
       <c r="C6" s="2">
-        <v>143.07000732421801</v>
+        <v>145.08999633789</v>
       </c>
       <c r="D6" s="2">
-        <v>145.08999633789</v>
+        <v>136.53999328613199</v>
       </c>
       <c r="E6" s="2">
-        <v>136.53999328613199</v>
+        <v>142.919998168945</v>
       </c>
       <c r="F6" s="2">
-        <v>142.919998168945</v>
+        <v>157611700</v>
       </c>
       <c r="G6" s="2">
-        <v>157611700</v>
-      </c>
-      <c r="H6" s="2">
         <v>142.46476745605401</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>22</v>
       </c>
-      <c r="B7" s="3">
-        <v>44218.270833333336</v>
+      <c r="B7" s="2">
+        <v>136.27999877929599</v>
       </c>
       <c r="C7" s="2">
-        <v>136.27999877929599</v>
+        <v>139.850006103515</v>
       </c>
       <c r="D7" s="2">
-        <v>139.850006103515</v>
+        <v>135.02000427246</v>
       </c>
       <c r="E7" s="2">
-        <v>135.02000427246</v>
+        <v>139.07000732421801</v>
       </c>
       <c r="F7" s="2">
-        <v>139.07000732421801</v>
+        <v>114459400</v>
       </c>
       <c r="G7" s="2">
-        <v>114459400</v>
-      </c>
-      <c r="H7" s="2">
         <v>138.627029418945</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21</v>
       </c>
-      <c r="B8" s="3">
-        <v>44217.270833333336</v>
+      <c r="B8" s="2">
+        <v>133.80000305175699</v>
       </c>
       <c r="C8" s="2">
-        <v>133.80000305175699</v>
+        <v>139.669998168945</v>
       </c>
       <c r="D8" s="2">
-        <v>139.669998168945</v>
+        <v>133.58999633789</v>
       </c>
       <c r="E8" s="2">
-        <v>133.58999633789</v>
+        <v>136.86999511718699</v>
       </c>
       <c r="F8" s="2">
-        <v>136.86999511718699</v>
+        <v>120150900</v>
       </c>
       <c r="G8" s="2">
-        <v>120150900</v>
-      </c>
-      <c r="H8" s="2">
         <v>136.43402099609301</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
-      <c r="B9" s="3">
-        <v>44216.270833333336</v>
+      <c r="B9" s="2">
+        <v>128.66000366210901</v>
       </c>
       <c r="C9" s="2">
-        <v>128.66000366210901</v>
+        <v>132.49000549316401</v>
       </c>
       <c r="D9" s="2">
-        <v>132.49000549316401</v>
+        <v>128.55000305175699</v>
       </c>
       <c r="E9" s="2">
-        <v>128.55000305175699</v>
+        <v>132.02999877929599</v>
       </c>
       <c r="F9" s="2">
-        <v>132.02999877929599</v>
+        <v>104319500</v>
       </c>
       <c r="G9" s="2">
-        <v>104319500</v>
-      </c>
-      <c r="H9" s="2">
         <v>131.609451293945</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
-        <v>44215.270833333336</v>
+      <c r="B10" s="2">
+        <v>127.77999877929599</v>
       </c>
       <c r="C10" s="2">
-        <v>127.77999877929599</v>
+        <v>128.71000671386699</v>
       </c>
       <c r="D10" s="2">
-        <v>128.71000671386699</v>
+        <v>126.94000244140599</v>
       </c>
       <c r="E10" s="2">
-        <v>126.94000244140599</v>
+        <v>127.83000183105401</v>
       </c>
       <c r="F10" s="2">
-        <v>127.83000183105401</v>
+        <v>90757300</v>
       </c>
       <c r="G10" s="2">
-        <v>90757300</v>
-      </c>
-      <c r="H10" s="2">
         <v>127.42282867431599</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
-        <v>44211.270833333336</v>
+      <c r="B11" s="2">
+        <v>128.77999877929599</v>
       </c>
       <c r="C11" s="2">
-        <v>128.77999877929599</v>
+        <v>130.22000122070301</v>
       </c>
       <c r="D11" s="2">
-        <v>130.22000122070301</v>
+        <v>127</v>
       </c>
       <c r="E11" s="2">
-        <v>127</v>
+        <v>127.139999389648</v>
       </c>
       <c r="F11" s="2">
-        <v>127.139999389648</v>
+        <v>111598500</v>
       </c>
       <c r="G11" s="2">
-        <v>111598500</v>
-      </c>
-      <c r="H11" s="2">
         <v>126.735023498535</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
-        <v>44210.270833333336</v>
+      <c r="B12" s="2">
+        <v>130.80000305175699</v>
       </c>
       <c r="C12" s="2">
-        <v>130.80000305175699</v>
+        <v>131</v>
       </c>
       <c r="D12" s="2">
-        <v>131</v>
+        <v>128.759994506835</v>
       </c>
       <c r="E12" s="2">
-        <v>128.759994506835</v>
+        <v>128.91000366210901</v>
       </c>
       <c r="F12" s="2">
-        <v>128.91000366210901</v>
+        <v>90221800</v>
       </c>
       <c r="G12" s="2">
-        <v>90221800</v>
-      </c>
-      <c r="H12" s="2">
         <v>128.49940490722599</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
-        <v>44209.270833333336</v>
+      <c r="B13" s="2">
+        <v>128.759994506835</v>
       </c>
       <c r="C13" s="2">
-        <v>128.759994506835</v>
+        <v>131.44999694824199</v>
       </c>
       <c r="D13" s="2">
-        <v>131.44999694824199</v>
+        <v>128.49000549316401</v>
       </c>
       <c r="E13" s="2">
-        <v>128.49000549316401</v>
+        <v>130.88999938964801</v>
       </c>
       <c r="F13" s="2">
-        <v>130.88999938964801</v>
+        <v>88636800</v>
       </c>
       <c r="G13" s="2">
-        <v>88636800</v>
-      </c>
-      <c r="H13" s="2">
         <v>130.47308349609301</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>44208.270833333336</v>
+      <c r="B14" s="2">
+        <v>128.5</v>
       </c>
       <c r="C14" s="2">
-        <v>128.5</v>
+        <v>129.69000244140599</v>
       </c>
       <c r="D14" s="2">
-        <v>129.69000244140599</v>
+        <v>126.86000061035099</v>
       </c>
       <c r="E14" s="2">
-        <v>126.86000061035099</v>
+        <v>128.80000305175699</v>
       </c>
       <c r="F14" s="2">
-        <v>128.80000305175699</v>
+        <v>91951100</v>
       </c>
       <c r="G14" s="2">
-        <v>91951100</v>
-      </c>
-      <c r="H14" s="2">
         <v>128.38973999023401</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="3">
-        <v>44207.270833333336</v>
+      <c r="B15" s="2">
+        <v>129.19000244140599</v>
       </c>
       <c r="C15" s="2">
-        <v>129.19000244140599</v>
+        <v>130.169998168945</v>
       </c>
       <c r="D15" s="2">
-        <v>130.169998168945</v>
+        <v>128.5</v>
       </c>
       <c r="E15" s="2">
-        <v>128.5</v>
+        <v>128.97999572753901</v>
       </c>
       <c r="F15" s="2">
-        <v>128.97999572753901</v>
+        <v>100384500</v>
       </c>
       <c r="G15" s="2">
-        <v>100384500</v>
-      </c>
-      <c r="H15" s="2">
         <v>128.56916809082</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" s="3">
-        <v>44204.270833333336</v>
+      <c r="B16" s="2">
+        <v>132.42999267578099</v>
       </c>
       <c r="C16" s="2">
-        <v>132.42999267578099</v>
+        <v>132.63000488281199</v>
       </c>
       <c r="D16" s="2">
-        <v>132.63000488281199</v>
+        <v>130.22999572753901</v>
       </c>
       <c r="E16" s="2">
-        <v>130.22999572753901</v>
+        <v>132.05000305175699</v>
       </c>
       <c r="F16" s="2">
-        <v>132.05000305175699</v>
+        <v>105158200</v>
       </c>
       <c r="G16" s="2">
-        <v>105158200</v>
-      </c>
-      <c r="H16" s="2">
         <v>131.62937927246</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>7</v>
       </c>
-      <c r="B17" s="3">
-        <v>44203.270833333336</v>
+      <c r="B17" s="2">
+        <v>128.36000061035099</v>
       </c>
       <c r="C17" s="2">
-        <v>128.36000061035099</v>
+        <v>131.63000488281199</v>
       </c>
       <c r="D17" s="2">
-        <v>131.63000488281199</v>
+        <v>127.86000061035099</v>
       </c>
       <c r="E17" s="2">
-        <v>127.86000061035099</v>
+        <v>130.919998168945</v>
       </c>
       <c r="F17" s="2">
-        <v>130.919998168945</v>
+        <v>109578200</v>
       </c>
       <c r="G17" s="2">
-        <v>109578200</v>
-      </c>
-      <c r="H17" s="2">
         <v>130.50299072265599</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" s="3">
-        <v>44202.270833333336</v>
+      <c r="B18" s="2">
+        <v>127.720001220703</v>
       </c>
       <c r="C18" s="2">
-        <v>127.720001220703</v>
+        <v>131.05000305175699</v>
       </c>
       <c r="D18" s="2">
-        <v>131.05000305175699</v>
+        <v>126.379997253417</v>
       </c>
       <c r="E18" s="2">
-        <v>126.379997253417</v>
+        <v>126.59999847412099</v>
       </c>
       <c r="F18" s="2">
-        <v>126.59999847412099</v>
+        <v>155088000</v>
       </c>
       <c r="G18" s="2">
-        <v>155088000</v>
-      </c>
-      <c r="H18" s="2">
         <v>126.19674682617099</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19" s="3">
-        <v>44201.270833333336</v>
+      <c r="B19" s="2">
+        <v>128.88999938964801</v>
       </c>
       <c r="C19" s="2">
-        <v>128.88999938964801</v>
+        <v>131.74000549316401</v>
       </c>
       <c r="D19" s="2">
-        <v>131.74000549316401</v>
+        <v>128.42999267578099</v>
       </c>
       <c r="E19" s="2">
-        <v>128.42999267578099</v>
+        <v>131.009994506835</v>
       </c>
       <c r="F19" s="2">
-        <v>131.009994506835</v>
+        <v>97664900</v>
       </c>
       <c r="G19" s="2">
-        <v>97664900</v>
-      </c>
-      <c r="H19" s="2">
         <v>130.59269714355401</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="3">
-        <v>44200.270833333336</v>
+      <c r="B20" s="2">
+        <v>133.52000427246</v>
       </c>
       <c r="C20" s="2">
-        <v>133.52000427246</v>
+        <v>133.61000061035099</v>
       </c>
       <c r="D20" s="2">
-        <v>133.61000061035099</v>
+        <v>126.76000213623</v>
       </c>
       <c r="E20" s="2">
-        <v>126.76000213623</v>
+        <v>129.41000366210901</v>
       </c>
       <c r="F20" s="2">
-        <v>129.41000366210901</v>
+        <v>143301900</v>
       </c>
       <c r="G20" s="2">
-        <v>143301900</v>
-      </c>
-      <c r="H20" s="2">
         <v>128.997802734375</v>
       </c>
     </row>

</xml_diff>